<commit_message>
making the integration for the zip and report part
</commit_message>
<xml_diff>
--- a/testData/urls.xlsx
+++ b/testData/urls.xlsx
@@ -11,26 +11,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.google.com/</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/</t>
+    <t>reportPath</t>
+  </si>
+  <si>
+    <t>folderPath</t>
+  </si>
+  <si>
+    <t>zipPath</t>
+  </si>
+  <si>
+    <t>senderEmail</t>
+  </si>
+  <si>
+    <t>senderPassword</t>
+  </si>
+  <si>
+    <t>recieverEmail</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>https://exa.unicen.edu.ar</t>
+  </si>
+  <si>
+    <t>generated_reports/lhreport.html</t>
+  </si>
+  <si>
+    <t>generated_reports</t>
+  </si>
+  <si>
+    <t>generated_reports/lhreports.zip</t>
+  </si>
+  <si>
+    <t>tt2857506@gmail.com</t>
+  </si>
+  <si>
+    <t>testtest2857506</t>
+  </si>
+  <si>
+    <t>ldemaio@solvd.com</t>
+  </si>
+  <si>
+    <t>lighthouse</t>
+  </si>
+  <si>
+    <t>Generated lighthouse report</t>
+  </si>
+  <si>
+    <t>https://google.com</t>
+  </si>
+  <si>
+    <t>testtest2857507</t>
+  </si>
+  <si>
+    <t>https://solvd.com</t>
+  </si>
+  <si>
+    <t>testtest2857508</t>
+  </si>
+  <si>
+    <t>https://reddit.com/</t>
+  </si>
+  <si>
+    <t>testtest2857509</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/</t>
+  </si>
+  <si>
+    <t>testtest2857510</t>
+  </si>
+  <si>
+    <t>https://www.cypress.io/</t>
+  </si>
+  <si>
+    <t>testtest2857511</t>
+  </si>
+  <si>
+    <t>https://twitter.com/</t>
+  </si>
+  <si>
+    <t>testtest2857512</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/web/tools/lighthouse</t>
+  </si>
+  <si>
+    <t>testtest2857513</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
     </font>
     <font>
       <color theme="1"/>
@@ -40,13 +130,27 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -63,6 +167,18 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -280,27 +396,290 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="25.71"/>
+    <col customWidth="1" min="2" max="2" width="28.29"/>
+    <col customWidth="1" min="3" max="3" width="16.57"/>
+    <col customWidth="1" min="4" max="4" width="27.86"/>
+    <col customWidth="1" min="5" max="5" width="20.57"/>
+    <col customWidth="1" min="6" max="6" width="15.29"/>
+    <col customWidth="1" min="7" max="7" width="18.43"/>
+    <col customWidth="1" min="8" max="8" width="11.29"/>
+    <col customWidth="1" min="9" max="9" width="24.71"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
     <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="A7"/>
+    <hyperlink r:id="rId7" ref="A8"/>
+    <hyperlink r:id="rId8" ref="A9"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Divide urls and emails data
</commit_message>
<xml_diff>
--- a/testData/urls.xlsx
+++ b/testData/urls.xlsx
@@ -11,34 +11,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
   <si>
+    <t>reportName</t>
+  </si>
+  <si>
     <t>https://www.google.com/</t>
   </si>
   <si>
+    <t>google_lhreport.html</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/</t>
+  </si>
+  <si>
+    <t>facebook_lhreport.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
-      <color theme="1"/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
+      <sz val="8.0"/>
+      <color rgb="FF103CC0"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -63,6 +76,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -280,20 +296,33 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="20.86"/>
+    <col customWidth="1" min="2" max="2" width="32.71"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>